<commit_message>
Add type to ulm parking spots
</commit_message>
<xml_diff>
--- a/sources/ulm_sensors.xlsx
+++ b/sources/ulm_sensors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\my-system-c\ipl\data\xlsx\ulm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3851F63-29B5-42AF-9D5B-DFCCDAE19575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA0FED6-3401-4248-ACB8-A9FED65B958D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52650" yWindow="4275" windowWidth="21345" windowHeight="15165" xr2:uid="{2FAF8A27-CC6F-4E11-A521-588849C98525}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2FAF8A27-CC6F-4E11-A521-588849C98525}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -152,9 +152,6 @@
     <t>Zweck der Anlage</t>
   </si>
   <si>
-    <t>C699C145-EB2E-4CF5-9A50-1A8A56FBF64D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Parkhaus Salzstadel                                                                                                                                                                                                                                            </t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>Auto</t>
   </si>
   <si>
-    <t>FD12A50D-0722-4A0A-AC47-CD88EFF6862A</t>
-  </si>
-  <si>
     <t xml:space="preserve">Parkhaus Deutschhaus                                                                                                                                                                                                                                           </t>
   </si>
   <si>
@@ -188,18 +182,12 @@
     <t>Friedrich-Ebert-Straße 8, 89073 Ulm</t>
   </si>
   <si>
-    <t>132BECEE-D7C9-441E-A76E-3ADB216A76BA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Parkhaus Fischerviertel                                                                                                                                                                                                                                        </t>
   </si>
   <si>
     <t>Schwilmengasse 1-1, 89073 Ulm</t>
   </si>
   <si>
-    <t>057786EF-EF3E-4837-A0B9-F8D609E9ED34</t>
-  </si>
-  <si>
     <t xml:space="preserve">Congresscentrum Nord                                                                                                                                                                                                                                           </t>
   </si>
   <si>
@@ -209,18 +197,12 @@
     <t>nein</t>
   </si>
   <si>
-    <t>6C5A1B0B-D83C-4C25-A4AF-4DB29D7280A8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Parkhaus am Rathaus                                                                                                                                                                                                                                            </t>
   </si>
   <si>
     <t>Neue Str., 89073 Ulm</t>
   </si>
   <si>
-    <t>FD6B8240-B9D2-4F85-B877-3EAE4E9B1C87</t>
-  </si>
-  <si>
     <t xml:space="preserve">Parkhaus Theater                                                                                                                                                                                                                                               </t>
   </si>
   <si>
@@ -233,7 +215,25 @@
     <t>Bahnhofplatz 8, 89073 Ulm</t>
   </si>
   <si>
-    <t>6173BA87-78EC-436C-85F0-B02C75C6B33B</t>
+    <t>c699c145-eb2e-4cf5-9a50-1a8a56fbf64d</t>
+  </si>
+  <si>
+    <t>fd12a50d-0722-4a0a-ac47-cd88eff6862a</t>
+  </si>
+  <si>
+    <t>132becee-d7c9-441e-a76e-3adb216a76ba</t>
+  </si>
+  <si>
+    <t>057786ef-ef3e-4837-a0b9-f8d609e9ed34</t>
+  </si>
+  <si>
+    <t>6c5a1b0b-d83c-4c25-a4af-4db29d7280a8</t>
+  </si>
+  <si>
+    <t>fd6b8240-b9d2-4f85-b877-3eae4e9b1c87</t>
+  </si>
+  <si>
+    <t>6173ba87-78ec-436c-85f0-b02c75c6b33b</t>
   </si>
 </sst>
 </file>
@@ -244,7 +244,7 @@
     <numFmt numFmtId="164" formatCode="0.0000000000000"/>
     <numFmt numFmtId="165" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +274,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -306,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -314,6 +319,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -669,16 +677,17 @@
   <dimension ref="A1:AD8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="106.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -768,18 +777,18 @@
       </c>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:30">
+      <c r="A2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
       </c>
       <c r="E2" s="3">
         <v>48.4011345561022</v>
@@ -788,7 +797,7 @@
         <v>9.9901596889959698</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2">
         <v>259200</v>
@@ -809,42 +818,42 @@
         <v>2</v>
       </c>
       <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="O2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="AB2">
         <v>2</v>
       </c>
       <c r="AC2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="3">
         <v>48.398085833722</v>
@@ -853,7 +862,7 @@
         <v>9.9847248686593399</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H3">
         <v>259200</v>
@@ -874,42 +883,42 @@
         <v>2</v>
       </c>
       <c r="N3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y3" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="O3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>34</v>
-      </c>
-      <c r="R3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="AB3">
         <v>2</v>
       </c>
       <c r="AC3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>41</v>
+    <row r="4" spans="1:30">
+      <c r="A4" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
       </c>
       <c r="E4" s="3">
         <v>48.396582769184</v>
@@ -918,7 +927,7 @@
         <v>9.9882761131336704</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H4">
         <v>604800</v>
@@ -939,42 +948,42 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y4" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="O4" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>34</v>
-      </c>
-      <c r="R4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="AB4">
         <v>2</v>
       </c>
       <c r="AC4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>44</v>
+    <row r="5" spans="1:30">
+      <c r="A5" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
       </c>
       <c r="E5" s="3">
         <v>48.401631838230998</v>
@@ -983,7 +992,7 @@
         <v>10.002430597494699</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I5">
         <v>410</v>
@@ -1001,19 +1010,19 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="S5" s="6">
         <v>0.27083333333333331</v>
@@ -1028,27 +1037,27 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB5">
         <v>2</v>
       </c>
       <c r="AC5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>48</v>
+    <row r="6" spans="1:30">
+      <c r="A6" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
         <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
       </c>
       <c r="E6" s="3">
         <v>48.397248418725397</v>
@@ -1057,7 +1066,7 @@
         <v>9.9909303974945196</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H6">
         <v>259200</v>
@@ -1078,42 +1087,42 @@
         <v>4</v>
       </c>
       <c r="N6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y6" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="O6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>34</v>
-      </c>
-      <c r="R6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y6" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="AB6">
         <v>2</v>
       </c>
       <c r="AC6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>51</v>
+    <row r="7" spans="1:30">
+      <c r="A7" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
       </c>
       <c r="E7" s="3">
         <v>48.4007540416262</v>
@@ -1122,7 +1131,7 @@
         <v>9.9855004541600998</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I7">
         <v>74</v>
@@ -1140,19 +1149,19 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="S7" s="6">
         <v>0.77083333333333337</v>
@@ -1173,27 +1182,27 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB7">
         <v>1.9</v>
       </c>
       <c r="AC7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:30">
+      <c r="A8" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
         <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
       </c>
       <c r="E8" s="3">
         <v>48.398229802932498</v>
@@ -1202,7 +1211,7 @@
         <v>9.9842604592319901</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H8">
         <v>604800</v>
@@ -1223,28 +1232,28 @@
         <v>8</v>
       </c>
       <c r="N8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y8" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="O8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y8" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="AB8">
         <v>2.2000000000000002</v>
       </c>
       <c r="AC8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix missing special parking capacities
</commit_message>
<xml_diff>
--- a/sources/ulm_sensors.xlsx
+++ b/sources/ulm_sensors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\my-system-c\ipl\data\xlsx\ulm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FTL\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA0FED6-3401-4248-ACB8-A9FED65B958D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139D158E-4716-4503-B3A4-5CAFDB91FBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2FAF8A27-CC6F-4E11-A521-588849C98525}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2FAF8A27-CC6F-4E11-A521-588849C98525}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -92,18 +92,6 @@
     <t>Anzahl Stellplätze</t>
   </si>
   <si>
-    <t>Anzahl Carsharing-Parkplätze</t>
-  </si>
-  <si>
-    <t>Anzahl Ladeplätze</t>
-  </si>
-  <si>
-    <t>Anzahl Frauenparkplätze</t>
-  </si>
-  <si>
-    <t>Anzahl Behindertenparkplätze</t>
-  </si>
-  <si>
     <t>Anlage beleuchtet?</t>
   </si>
   <si>
@@ -234,6 +222,18 @@
   </si>
   <si>
     <t>6173ba87-78ec-436c-85f0-b02c75c6b33b</t>
+  </si>
+  <si>
+    <t>Anzahl Stellplätze Carsharing</t>
+  </si>
+  <si>
+    <t>Anzahl Stellplätze Lademöglichkeit</t>
+  </si>
+  <si>
+    <t>Anzahl Stellplätze Frauen</t>
+  </si>
+  <si>
+    <t>Anzahl Stellplätze Behinderte</t>
   </si>
 </sst>
 </file>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54411EF9-4ECD-406D-85AB-8CEFA9039220}">
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -685,6 +685,8 @@
     <col min="1" max="1" width="38.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="106.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -716,79 +718,79 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="AD1" s="1"/>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E2" s="3">
         <v>48.4011345561022</v>
@@ -797,7 +799,7 @@
         <v>9.9901596889959698</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H2">
         <v>259200</v>
@@ -818,42 +820,42 @@
         <v>2</v>
       </c>
       <c r="N2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="P2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="R2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AB2">
         <v>2</v>
       </c>
       <c r="AC2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3">
         <v>48.398085833722</v>
@@ -862,7 +864,7 @@
         <v>9.9847248686593399</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H3">
         <v>259200</v>
@@ -883,42 +885,42 @@
         <v>2</v>
       </c>
       <c r="N3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="P3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Q3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="R3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AB3">
         <v>2</v>
       </c>
       <c r="AC3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:30">
       <c r="A4" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E4" s="3">
         <v>48.396582769184</v>
@@ -927,7 +929,7 @@
         <v>9.9882761131336704</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H4">
         <v>604800</v>
@@ -948,42 +950,42 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="P4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Q4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="R4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AB4">
         <v>2</v>
       </c>
       <c r="AC4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:30">
       <c r="A5" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E5" s="3">
         <v>48.401631838230998</v>
@@ -992,7 +994,7 @@
         <v>10.002430597494699</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I5">
         <v>410</v>
@@ -1010,19 +1012,19 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="P5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Q5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="R5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S5" s="6">
         <v>0.27083333333333331</v>
@@ -1037,27 +1039,27 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AB5">
         <v>2</v>
       </c>
       <c r="AC5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E6" s="3">
         <v>48.397248418725397</v>
@@ -1066,7 +1068,7 @@
         <v>9.9909303974945196</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H6">
         <v>259200</v>
@@ -1087,42 +1089,42 @@
         <v>4</v>
       </c>
       <c r="N6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="P6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Q6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="R6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AB6">
         <v>2</v>
       </c>
       <c r="AC6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3">
         <v>48.4007540416262</v>
@@ -1131,7 +1133,7 @@
         <v>9.9855004541600998</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I7">
         <v>74</v>
@@ -1149,19 +1151,19 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="P7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Q7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="R7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S7" s="6">
         <v>0.77083333333333337</v>
@@ -1182,27 +1184,27 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AB7">
         <v>1.9</v>
       </c>
       <c r="AC7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3">
         <v>48.398229802932498</v>
@@ -1211,7 +1213,7 @@
         <v>9.9842604592319901</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H8">
         <v>604800</v>
@@ -1232,28 +1234,28 @@
         <v>8</v>
       </c>
       <c r="N8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="P8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Q8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="R8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AB8">
         <v>2.2000000000000002</v>
       </c>
       <c r="AC8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1294,6 +1296,7 @@
     <hyperlink ref="Y2" r:id="rId7" xr:uid="{66C616E0-960A-460B-B9A8-AC092D53239B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>